<commit_message>
100 mhz clock designs
</commit_message>
<xml_diff>
--- a/dtpu_configurations/only_integer8/100mhz/mxu_10x10/timing.xlsx
+++ b/dtpu_configurations/only_integer8/100mhz/mxu_10x10/timing.xlsx
@@ -99,7 +99,7 @@
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
     <col min="1" max="1" width="51.40625" customWidth="true"/>
-    <col min="2" max="2" width="10.0" customWidth="true"/>
+    <col min="2" max="2" width="8.75" customWidth="true"/>
     <col min="3" max="3" width="8.75" customWidth="true"/>
   </cols>
   <sheetData>
@@ -119,10 +119,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="n" s="4">
-        <v>17.5273494720459</v>
+        <v>0.6887282133102417</v>
       </c>
       <c r="C2" t="n" s="4">
-        <v>0.007638223469257355</v>
+        <v>0.010574874468147755</v>
       </c>
     </row>
   </sheetData>

</xml_diff>